<commit_message>
Inicio projeto SP Medical Group
</commit_message>
<xml_diff>
--- a/Projeto Gufi/Fisico-projeto-gufi.xlsx
+++ b/Projeto Gufi/Fisico-projeto-gufi.xlsx
@@ -51,9 +51,6 @@
     <t>Escola Senai de Informatica</t>
   </si>
   <si>
-    <t>A. Barão de Limeira, 538</t>
-  </si>
-  <si>
     <t>idUsuario</t>
   </si>
   <si>
@@ -160,6 +157,9 @@
   </si>
   <si>
     <t>confirmada</t>
+  </si>
+  <si>
+    <t>Al. Barão de Limeira, 538</t>
   </si>
 </sst>
 </file>
@@ -314,70 +314,70 @@
   </cellStyleXfs>
   <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -695,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="D6" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -712,365 +712,365 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="E2" s="4" t="s">
+      <c r="C2" s="18"/>
+      <c r="E2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="3">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="7">
-        <v>1</v>
-      </c>
-      <c r="F4" s="7">
+      <c r="E4" s="5">
+        <v>1</v>
+      </c>
+      <c r="F4" s="5">
         <v>99999999999</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="2">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="3">
+      <c r="C8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="7">
+        <v>1</v>
+      </c>
+      <c r="C9" s="7">
+        <v>1</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="7">
         <v>2</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="8" t="s">
+      <c r="C10" s="7">
+        <v>2</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="10">
-        <v>1</v>
-      </c>
-      <c r="C9" s="10">
-        <v>1</v>
-      </c>
-      <c r="D9" s="10" t="s">
+      <c r="E10" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="7">
         <v>3</v>
       </c>
-      <c r="E9" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="10">
+      <c r="C11" s="7">
         <v>2</v>
       </c>
-      <c r="C10" s="10">
+      <c r="D11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="21"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="10">
+        <v>1</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="10">
         <v>2</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="10">
+      <c r="C16" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="10">
         <v>3</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C17" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="16"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H20" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="22"/>
+      <c r="L20" s="22"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="12">
+        <v>1</v>
+      </c>
+      <c r="C21" s="12">
+        <v>1</v>
+      </c>
+      <c r="D21" s="12">
+        <v>1</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F21" s="12">
+        <v>1</v>
+      </c>
+      <c r="G21" s="13">
+        <v>44293</v>
+      </c>
+      <c r="H21" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="12">
         <v>2</v>
       </c>
-      <c r="D11" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="12"/>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="14">
-        <v>1</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="14">
+      <c r="C22" s="12">
         <v>2</v>
       </c>
-      <c r="C16" s="14" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="14">
+      <c r="D22" s="12">
+        <v>1</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F22" s="12">
+        <v>0</v>
+      </c>
+      <c r="G22" s="13">
+        <v>44294</v>
+      </c>
+      <c r="H22" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B23" s="12">
         <v>3</v>
       </c>
-      <c r="C17" s="14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="15" t="s">
+      <c r="C23" s="12">
+        <v>3</v>
+      </c>
+      <c r="D23" s="12">
+        <v>1</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F23" s="12">
+        <v>1</v>
+      </c>
+      <c r="G23" s="13">
+        <v>44295</v>
+      </c>
+      <c r="H23" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="15"/>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E20" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="F20" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="G20" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="H20" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="I20" s="17"/>
-      <c r="J20" s="17"/>
-      <c r="K20" s="17"/>
-      <c r="L20" s="17"/>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="18">
-        <v>1</v>
-      </c>
-      <c r="C21" s="18">
-        <v>1</v>
-      </c>
-      <c r="D21" s="18">
-        <v>1</v>
-      </c>
-      <c r="E21" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="F21" s="18">
-        <v>1</v>
-      </c>
-      <c r="G21" s="19">
-        <v>44293</v>
-      </c>
-      <c r="H21" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="I21" s="20"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="20"/>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="18">
+      <c r="E26" s="14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B27" s="3">
+        <v>1</v>
+      </c>
+      <c r="C27" s="3">
         <v>2</v>
       </c>
-      <c r="C22" s="18">
+      <c r="D27" s="3">
         <v>2</v>
       </c>
-      <c r="D22" s="18">
-        <v>1</v>
-      </c>
-      <c r="E22" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F22" s="18">
-        <v>0</v>
-      </c>
-      <c r="G22" s="19">
-        <v>44294</v>
-      </c>
-      <c r="H22" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="I22" s="20"/>
-      <c r="J22" s="20"/>
-      <c r="K22" s="20"/>
-      <c r="L22" s="20"/>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="18">
+      <c r="E27" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B28" s="3">
+        <v>2</v>
+      </c>
+      <c r="C28" s="3">
+        <v>2</v>
+      </c>
+      <c r="D28" s="3">
         <v>3</v>
       </c>
-      <c r="C23" s="18">
+      <c r="E28" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B29" s="3">
         <v>3</v>
       </c>
-      <c r="D23" s="18">
-        <v>1</v>
-      </c>
-      <c r="E23" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F23" s="18">
-        <v>1</v>
-      </c>
-      <c r="G23" s="19">
-        <v>44295</v>
-      </c>
-      <c r="H23" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="20"/>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="C26" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="D26" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="E26" s="22" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B27" s="5">
-        <v>1</v>
-      </c>
-      <c r="C27" s="5">
-        <v>2</v>
-      </c>
-      <c r="D27" s="5">
-        <v>2</v>
-      </c>
-      <c r="E27" s="5" t="s">
+      <c r="C29" s="3">
+        <v>3</v>
+      </c>
+      <c r="D29" s="3">
+        <v>1</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B28" s="5">
-        <v>2</v>
-      </c>
-      <c r="C28" s="5">
-        <v>2</v>
-      </c>
-      <c r="D28" s="5">
-        <v>3</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B29" s="5">
-        <v>3</v>
-      </c>
-      <c r="C29" s="5">
-        <v>3</v>
-      </c>
-      <c r="D29" s="5">
-        <v>1</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>